<commit_message>
Q3 and Q4 commit1.1
</commit_message>
<xml_diff>
--- a/Arrays/Arrays Questions.xlsx
+++ b/Arrays/Arrays Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLTUser\Desktop\DSA\Arrays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E357BBC8-9F7B-4002-B1BC-992992FCD8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2467894F-2BAF-4F32-93D8-1CF208EDE68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{78EDE833-7929-4DDD-82CF-287672B52B0D}"/>
   </bookViews>
@@ -1043,7 +1043,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1113,6 +1113,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Bahnschrift SemiCondensed"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Bahnschrift"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1202,7 +1208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1243,11 +1249,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1741,7 +1768,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1789,21 +1816,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>10</v>
@@ -1820,19 +1847,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>15</v>
@@ -1841,24 +1868,24 @@
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>15</v>
@@ -2060,50 +2087,55 @@
       <c r="J13" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:J10">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="A3:J3 B2:J2 A5:J10 B4:J4">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:J12 A11:A13 B13 E13:J13">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>$B11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:D13">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>$B12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Partially Correct"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Answered"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Wrong"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H13">
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
       <formula>"Partially Correct"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>"Answered"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>$B2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H13" xr:uid="{35DB0175-A1CD-4EED-B45E-E094B62AF3FE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H13 H1:H4" xr:uid="{35DB0175-A1CD-4EED-B45E-E094B62AF3FE}">
       <formula1>"Answered, Partially Correct, Wrong"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G13" xr:uid="{EB63211C-D221-4711-8B4B-66BBF46BA3D2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G13 G1:G4" xr:uid="{EB63211C-D221-4711-8B4B-66BBF46BA3D2}">
       <formula1>"Very Easy, Easy, Medium, Medium-Hard, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J13" xr:uid="{B93DF45A-2457-43E8-8596-1D9AB55A40F5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J13 J2:J4" xr:uid="{B93DF45A-2457-43E8-8596-1D9AB55A40F5}">
       <formula1>"Jan, Feb, March, April, May, June, July, Aug, Sept, Oct, Nov, Dec"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>